<commit_message>
Spreadsheet updated to 1.33x for corvs/frigs
</commit_message>
<xml_diff>
--- a/Balance Info/HW1 Ideal Design.xlsx
+++ b/Balance Info/HW1 Ideal Design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="323">
   <si>
     <t>Hiig</t>
   </si>
@@ -595,9 +595,6 @@
     <t>pulse</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>same</t>
   </si>
   <si>
@@ -1007,6 +1004,9 @@
   </si>
   <si>
     <t>Ideal Time (1-&gt;2 res)</t>
+  </si>
+  <si>
+    <t>15?</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
@@ -1440,19 +1440,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E37">
         <v>575</v>
@@ -1802,7 +1802,7 @@
         <v>1.3</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E40">
         <v>85</v>
@@ -1820,7 +1820,7 @@
         <v>800</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E41">
         <v>500</v>
@@ -1848,7 +1848,7 @@
         <v>1.2</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E44">
         <v>65</v>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E60">
         <v>800</v>
@@ -2031,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E63">
         <v>240</v>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E65">
         <v>55</v>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E66">
         <v>650</v>
@@ -2105,7 +2105,7 @@
         <v>0.9375</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E67">
         <v>135</v>
@@ -2127,7 +2127,7 @@
         <v>1.1458333333333333</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E68">
         <v>275</v>
@@ -2165,7 +2165,7 @@
         <v>0.97916666666666663</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E71">
         <v>225</v>
@@ -2203,7 +2203,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E74">
         <v>150</v>
@@ -2221,7 +2221,7 @@
         <v>600</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E75">
         <v>700</v>
@@ -2275,7 +2275,7 @@
         <v>600</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E81">
         <v>650</v>
@@ -2289,7 +2289,7 @@
         <v>900</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E82">
         <v>680</v>
@@ -2307,7 +2307,7 @@
         <v>1.0416666666666667</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E83">
         <v>220</v>
@@ -2329,7 +2329,7 @@
         <v>0.7</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E84">
         <v>35</v>
@@ -2347,7 +2347,7 @@
         <v>700</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E85">
         <v>800</v>
@@ -2365,7 +2365,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E86">
         <v>425</v>
@@ -2435,7 +2435,7 @@
         <v>1.3</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E93">
         <v>85</v>
@@ -2465,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E95">
         <v>800</v>
@@ -3019,7 +3019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3035,13 +3035,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>177</v>
@@ -3348,7 +3348,7 @@
         <v>68</v>
       </c>
       <c r="C37" s="5">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D37" s="8">
         <v>60</v>
@@ -3385,7 +3385,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" s="8">
         <v>20</v>
@@ -3436,8 +3436,8 @@
       <c r="B40">
         <v>15</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>185</v>
+      <c r="C40" s="5" t="s">
+        <v>322</v>
       </c>
       <c r="D40" s="8">
         <v>45</v>
@@ -3496,7 +3496,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D44" s="8">
         <v>9</v>
@@ -3534,7 +3534,7 @@
         <v>145</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D45" s="8">
         <v>150</v>
@@ -3674,7 +3674,7 @@
         <v>77</v>
       </c>
       <c r="C60" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D60" s="8">
         <v>75</v>
@@ -3725,8 +3725,8 @@
       <c r="B63" s="2">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
-        <v>19</v>
+      <c r="C63" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="D63" s="8">
         <v>25</v>
@@ -3763,7 +3763,7 @@
         <v>250</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D64" s="8">
         <v>420</v>
@@ -3814,7 +3814,7 @@
         <v>73</v>
       </c>
       <c r="C66" s="5">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D66" s="8">
         <v>60</v>
@@ -3851,8 +3851,8 @@
       <c r="B67">
         <v>18</v>
       </c>
-      <c r="C67" s="5">
-        <v>17</v>
+      <c r="C67" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="D67" s="8">
         <v>22</v>
@@ -3890,7 +3890,7 @@
         <v>25</v>
       </c>
       <c r="C68" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D68" s="8">
         <v>40</v>
@@ -3928,7 +3928,7 @@
         <v>160</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D69" s="8">
         <v>175</v>
@@ -3942,7 +3942,7 @@
         <v>300</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D70" s="8">
         <v>300</v>
@@ -3955,8 +3955,8 @@
       <c r="B71" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C71" s="5">
-        <v>21</v>
+      <c r="C71" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="D71" s="8">
         <v>28</v>
@@ -4012,7 +4012,7 @@
         <v>20</v>
       </c>
       <c r="C74" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D74" s="8">
         <v>20</v>
@@ -4128,7 +4128,7 @@
         <v>30</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D83" s="8">
         <v>30</v>
@@ -4213,7 +4213,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="5">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D86" s="8">
         <v>65</v>
@@ -4259,7 +4259,7 @@
         <v>68</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D88" s="8"/>
     </row>
@@ -4271,7 +4271,7 @@
         <v>10</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D89" s="8"/>
     </row>
@@ -4283,7 +4283,7 @@
         <v>210</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>60</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D91" s="8"/>
     </row>
@@ -4306,7 +4306,7 @@
         <v>9</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D92" s="8"/>
     </row>
@@ -4317,8 +4317,8 @@
       <c r="B93">
         <v>18</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>185</v>
+      <c r="C93" s="5" t="s">
+        <v>322</v>
       </c>
       <c r="D93" s="8">
         <v>20</v>
@@ -4356,7 +4356,7 @@
         <v>145</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D94" s="8"/>
     </row>
@@ -4368,7 +4368,7 @@
         <v>77</v>
       </c>
       <c r="C95" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D95" s="8">
         <v>75</v>
@@ -4405,7 +4405,7 @@
         <v>600</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D96" s="8"/>
     </row>
@@ -4417,7 +4417,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D97" s="8"/>
     </row>
@@ -4429,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D98" s="8"/>
     </row>
@@ -4441,7 +4441,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D99" s="8"/>
     </row>
@@ -4453,7 +4453,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D100" s="8"/>
     </row>
@@ -4465,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D101" s="8"/>
     </row>
@@ -4477,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D102" s="8"/>
     </row>
@@ -4489,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D103" s="8"/>
     </row>
@@ -4501,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D104" s="8"/>
     </row>
@@ -4513,7 +4513,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D105" s="8"/>
     </row>
@@ -4525,7 +4525,7 @@
         <v>60</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D106" s="8"/>
     </row>
@@ -4534,7 +4534,7 @@
         <v>108</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D107" s="8"/>
     </row>
@@ -4546,7 +4546,7 @@
         <v>20</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D108" s="8"/>
     </row>
@@ -4558,7 +4558,7 @@
         <v>250</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D109" s="8"/>
     </row>
@@ -4570,7 +4570,7 @@
         <v>7</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D110" s="8"/>
     </row>
@@ -4582,7 +4582,7 @@
         <v>73</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D111" s="8"/>
     </row>
@@ -4594,7 +4594,7 @@
         <v>18</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D112" s="8"/>
     </row>
@@ -4606,7 +4606,7 @@
         <v>25</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D113" s="8"/>
     </row>
@@ -4618,7 +4618,7 @@
         <v>160</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D114" s="8"/>
     </row>
@@ -4630,7 +4630,7 @@
         <v>300</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D115" s="8"/>
     </row>
@@ -4642,7 +4642,7 @@
         <v>22</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D116" s="8"/>
     </row>
@@ -4654,7 +4654,7 @@
         <v>15</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D117" s="8"/>
     </row>
@@ -4666,7 +4666,7 @@
         <v>15</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D118" s="8"/>
     </row>
@@ -4678,7 +4678,7 @@
         <v>20</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D119" s="8"/>
     </row>
@@ -4690,7 +4690,7 @@
         <v>50</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D120" s="8"/>
     </row>
@@ -4702,7 +4702,7 @@
         <v>45</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D121" s="8"/>
     </row>
@@ -4714,7 +4714,7 @@
         <v>45</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D122" s="8"/>
     </row>
@@ -4726,7 +4726,7 @@
         <v>45</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D123" s="8"/>
     </row>
@@ -4738,7 +4738,7 @@
         <v>45</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D124" s="8"/>
     </row>
@@ -4750,7 +4750,7 @@
         <v>45</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D125" s="8"/>
     </row>
@@ -4762,7 +4762,7 @@
         <v>600</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D126" s="8"/>
     </row>
@@ -4774,7 +4774,7 @@
         <v>50</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D127" s="8"/>
     </row>
@@ -4786,7 +4786,7 @@
         <v>60</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D128" s="8"/>
     </row>
@@ -4798,7 +4798,7 @@
         <v>30</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D129" s="8"/>
     </row>
@@ -4810,7 +4810,7 @@
         <v>10</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D130" s="8"/>
     </row>
@@ -4822,7 +4822,7 @@
         <v>70</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D131" s="8"/>
     </row>
@@ -4834,7 +4834,7 @@
         <v>85</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D132" s="8"/>
     </row>
@@ -4846,7 +4846,7 @@
         <v>1</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D133" s="8"/>
     </row>
@@ -5105,7 +5105,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5132,37 +5132,37 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5798,7 +5798,7 @@
         <v>1.0576923076923077</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K37" s="8">
         <v>16000</v>
@@ -5829,7 +5829,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K38" s="8">
         <v>110</v>
@@ -5860,7 +5860,7 @@
         <v>0.99056603773584906</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K39" s="8">
         <v>72000</v>
@@ -5892,7 +5892,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K40" s="8">
         <v>150</v>
@@ -6026,7 +6026,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K45" s="8">
         <v>44000</v>
@@ -6379,7 +6379,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K63" s="8">
         <v>1700</v>
@@ -6410,7 +6410,7 @@
         <v>2.2641509433962264</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K64" s="8">
         <v>90000</v>
@@ -6442,7 +6442,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K65" s="8">
         <v>160</v>
@@ -6473,7 +6473,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K66" s="8">
         <v>15000</v>
@@ -6504,7 +6504,7 @@
         <v>0.52941176470588236</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K67" s="8">
         <v>900</v>
@@ -6535,7 +6535,7 @@
         <v>0.63529411764705879</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H68" s="5">
         <v>1080</v>
@@ -6676,10 +6676,10 @@
         <v>1</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -6699,10 +6699,10 @@
         <v>1</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -6729,7 +6729,7 @@
         <v>1200</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I74" s="5">
         <v>1</v>
@@ -6762,13 +6762,13 @@
         <v>1</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K75" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L75" t="s">
         <v>212</v>
-      </c>
-      <c r="L75" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -6876,7 +6876,7 @@
         <v>5000</v>
       </c>
       <c r="K81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -6905,7 +6905,7 @@
         <v>1</v>
       </c>
       <c r="K82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -6929,7 +6929,7 @@
         <v>0.58823529411764708</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K83" s="8">
         <v>1500</v>
@@ -6960,7 +6960,7 @@
         <v>0.44444444444444442</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K84" s="8">
         <v>110</v>
@@ -6987,7 +6987,7 @@
         <v>1</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K85" s="8">
         <v>4500</v>
@@ -7014,7 +7014,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K86" s="8">
         <v>12000</v>
@@ -7058,7 +7058,7 @@
         <v>1.2</v>
       </c>
       <c r="G88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -7078,7 +7078,7 @@
         <v>1</v>
       </c>
       <c r="G89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -7098,7 +7098,7 @@
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -7118,7 +7118,7 @@
         <v>1.2</v>
       </c>
       <c r="G91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -7138,7 +7138,7 @@
         <v>0.9</v>
       </c>
       <c r="G92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -7195,7 +7195,7 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -7256,7 +7256,7 @@
         <v>1.2</v>
       </c>
       <c r="G96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -7276,7 +7276,7 @@
         <v>0.01</v>
       </c>
       <c r="G97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -7296,7 +7296,7 @@
         <v>0.5</v>
       </c>
       <c r="G98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -7316,7 +7316,7 @@
         <v>0.5</v>
       </c>
       <c r="G99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -7336,7 +7336,7 @@
         <v>0.5</v>
       </c>
       <c r="G100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -7356,7 +7356,7 @@
         <v>0.5</v>
       </c>
       <c r="G101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -7376,7 +7376,7 @@
         <v>0.5</v>
       </c>
       <c r="G102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -7396,7 +7396,7 @@
         <v>0.5</v>
       </c>
       <c r="G103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -7416,7 +7416,7 @@
         <v>0.5</v>
       </c>
       <c r="G104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -7436,7 +7436,7 @@
         <v>0.5</v>
       </c>
       <c r="G105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -7456,7 +7456,7 @@
         <v>1.2</v>
       </c>
       <c r="G106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -7476,7 +7476,7 @@
         <v>1</v>
       </c>
       <c r="G107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -7496,7 +7496,7 @@
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -7516,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -7536,7 +7536,7 @@
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -7556,7 +7556,7 @@
         <v>1.2</v>
       </c>
       <c r="G111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -7576,7 +7576,7 @@
         <v>1</v>
       </c>
       <c r="G112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -7596,7 +7596,7 @@
         <v>0.8</v>
       </c>
       <c r="G113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -7616,7 +7616,7 @@
         <v>1</v>
       </c>
       <c r="G114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -7636,7 +7636,7 @@
         <v>0.85</v>
       </c>
       <c r="G115" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -7656,7 +7656,7 @@
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -7676,7 +7676,7 @@
         <v>1</v>
       </c>
       <c r="G117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -7696,7 +7696,7 @@
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -7716,7 +7716,7 @@
         <v>0.8</v>
       </c>
       <c r="G119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -7736,7 +7736,7 @@
         <v>1</v>
       </c>
       <c r="G120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -7756,7 +7756,7 @@
         <v>1</v>
       </c>
       <c r="G121" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -7776,7 +7776,7 @@
         <v>1</v>
       </c>
       <c r="G122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -7796,7 +7796,7 @@
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -7816,7 +7816,7 @@
         <v>1</v>
       </c>
       <c r="G124" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -7836,7 +7836,7 @@
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -7856,7 +7856,7 @@
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -7876,7 +7876,7 @@
         <v>1</v>
       </c>
       <c r="G127" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -7896,7 +7896,7 @@
         <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -7916,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -7936,7 +7936,7 @@
         <v>1</v>
       </c>
       <c r="G130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -7956,7 +7956,7 @@
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -7976,7 +7976,7 @@
         <v>1.2</v>
       </c>
       <c r="G132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -7996,7 +7996,7 @@
         <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -8527,28 +8527,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>321</v>
-      </c>
       <c r="I1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -8560,7 +8560,7 @@
         <v>135</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8577,7 +8577,7 @@
         <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8588,7 +8588,7 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8609,7 +8609,7 @@
         <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8621,7 +8621,7 @@
         <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -8633,7 +8633,7 @@
         <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -8679,7 +8679,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -8691,7 +8691,7 @@
         <v>225</v>
       </c>
       <c r="E19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -8708,7 +8708,7 @@
         <v>225</v>
       </c>
       <c r="E21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -8725,7 +8725,7 @@
         <v>248</v>
       </c>
       <c r="E23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -8755,7 +8755,7 @@
         <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -8805,7 +8805,7 @@
         <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -8826,7 +8826,7 @@
         <v>190</v>
       </c>
       <c r="E37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F37" s="5">
         <v>160</v>
@@ -8841,7 +8841,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F38" s="5">
         <v>80</v>
@@ -8860,7 +8860,7 @@
         <v>248</v>
       </c>
       <c r="E39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F39" s="5">
         <v>200</v>
@@ -8875,7 +8875,7 @@
         <v>181</v>
       </c>
       <c r="E40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F40" s="5">
         <v>150</v>
@@ -8905,7 +8905,7 @@
         <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F44" s="5">
         <v>110</v>
@@ -8924,7 +8924,7 @@
         <v>369</v>
       </c>
       <c r="E45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F45" s="5">
         <v>390</v>
@@ -9013,7 +9013,7 @@
         <v>213</v>
       </c>
       <c r="E60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F60" s="5">
         <v>220</v>
@@ -9042,7 +9042,7 @@
         <v>185</v>
       </c>
       <c r="E63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F63" s="5">
         <v>160</v>
@@ -9061,7 +9061,7 @@
         <v>577</v>
       </c>
       <c r="E64" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F64" s="5">
         <v>645</v>
@@ -9076,7 +9076,7 @@
         <v>110</v>
       </c>
       <c r="E65" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F65" s="5">
         <v>80</v>
@@ -9095,7 +9095,7 @@
         <v>242</v>
       </c>
       <c r="E66" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F66" s="5">
         <v>250</v>
@@ -9114,7 +9114,7 @@
         <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F67" s="5">
         <v>100</v>
@@ -9133,7 +9133,7 @@
         <v>213</v>
       </c>
       <c r="E68" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F68" s="5">
         <v>210</v>
@@ -9152,7 +9152,7 @@
         <v>283</v>
       </c>
       <c r="E69" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F69" s="5">
         <v>270</v>
@@ -9179,7 +9179,7 @@
         <v>187</v>
       </c>
       <c r="E71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F71" s="5">
         <v>170</v>
@@ -9262,7 +9262,7 @@
         <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F83" s="5">
         <v>140</v>
@@ -9297,7 +9297,7 @@
         <v>121</v>
       </c>
       <c r="E86" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F86" s="5">
         <v>100</v>
@@ -9313,7 +9313,7 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -9321,7 +9321,7 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -9329,7 +9329,7 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -9337,7 +9337,7 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -9345,7 +9345,7 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -9357,7 +9357,7 @@
         <v>181</v>
       </c>
       <c r="E93" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F93" s="5">
         <v>150</v>
@@ -9368,7 +9368,7 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -9384,7 +9384,7 @@
         <v>213</v>
       </c>
       <c r="E95" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F95" s="5">
         <v>220</v>
@@ -9395,7 +9395,7 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -9403,7 +9403,7 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -9411,7 +9411,7 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -9419,7 +9419,7 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -9427,7 +9427,7 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -9435,7 +9435,7 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -9443,7 +9443,7 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -9451,7 +9451,7 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -9459,7 +9459,7 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -9467,7 +9467,7 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -9475,7 +9475,7 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -9483,7 +9483,7 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -9491,7 +9491,7 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -9499,7 +9499,7 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -9507,7 +9507,7 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -9515,7 +9515,7 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -9523,7 +9523,7 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -9531,7 +9531,7 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -9539,7 +9539,7 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -9547,7 +9547,7 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -9555,7 +9555,7 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -9563,7 +9563,7 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -9571,7 +9571,7 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -9579,7 +9579,7 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -9587,7 +9587,7 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -9595,7 +9595,7 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -9603,7 +9603,7 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -9611,7 +9611,7 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -9619,7 +9619,7 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -9627,7 +9627,7 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -9635,7 +9635,7 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -9643,7 +9643,7 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -9651,7 +9651,7 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -9659,7 +9659,7 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -9667,7 +9667,7 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -9675,7 +9675,7 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -9683,7 +9683,7 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -9691,7 +9691,7 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -9703,7 +9703,7 @@
         <v>212</v>
       </c>
       <c r="E134" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -9720,7 +9720,7 @@
         <v>63</v>
       </c>
       <c r="E136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -9731,7 +9731,7 @@
         <v>70</v>
       </c>
       <c r="E137" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -9743,7 +9743,7 @@
         <v>160</v>
       </c>
       <c r="E138" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -9760,7 +9760,7 @@
         <v>169</v>
       </c>
       <c r="E140" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -9772,7 +9772,7 @@
         <v>180</v>
       </c>
       <c r="E141" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -9789,7 +9789,7 @@
         <v>222</v>
       </c>
       <c r="E143" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -9800,7 +9800,7 @@
         <v>45</v>
       </c>
       <c r="E144" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -9812,7 +9812,7 @@
         <v>63</v>
       </c>
       <c r="E145" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -9824,7 +9824,7 @@
         <v>160</v>
       </c>
       <c r="E146" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -9836,7 +9836,7 @@
         <v>188</v>
       </c>
       <c r="E147" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -9848,7 +9848,7 @@
         <v>118</v>
       </c>
       <c r="E148" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -9951,60 +9951,60 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>265</v>
-      </c>
       <c r="E1" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="N1" t="s">
         <v>313</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="O1" t="s">
         <v>312</v>
       </c>
-      <c r="L1" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="P1" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="N1" t="s">
-        <v>314</v>
-      </c>
-      <c r="O1" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" t="s">
         <v>239</v>
-      </c>
-      <c r="B2" t="s">
-        <v>240</v>
       </c>
       <c r="C2" s="18">
         <v>100</v>
@@ -10052,15 +10052,15 @@
         <v>18.75</v>
       </c>
       <c r="Q2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
         <v>237</v>
-      </c>
-      <c r="B3" t="s">
-        <v>238</v>
       </c>
       <c r="C3" s="18">
         <v>200</v>
@@ -10110,10 +10110,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
         <v>231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>232</v>
       </c>
       <c r="C4" s="18">
         <v>400</v>
@@ -10163,10 +10163,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" s="18">
         <v>500</v>
@@ -10184,7 +10184,7 @@
         <v>50</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J5" s="19" t="str">
         <f t="shared" si="0"/>
@@ -10216,10 +10216,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="18">
         <v>500</v>
@@ -10237,7 +10237,7 @@
         <v>50</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J6" s="19" t="str">
         <f t="shared" si="0"/>
@@ -10269,10 +10269,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" t="s">
         <v>229</v>
-      </c>
-      <c r="B7" t="s">
-        <v>230</v>
       </c>
       <c r="C7" s="18">
         <v>800</v>
@@ -10322,10 +10322,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
         <v>227</v>
-      </c>
-      <c r="B8" t="s">
-        <v>228</v>
       </c>
       <c r="C8" s="18">
         <v>900</v>
@@ -10375,16 +10375,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" t="s">
         <v>245</v>
-      </c>
-      <c r="B9" t="s">
-        <v>246</v>
       </c>
       <c r="C9" s="18">
         <v>600</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E9" s="21">
         <v>14</v>
@@ -10428,16 +10428,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
         <v>235</v>
-      </c>
-      <c r="B10" t="s">
-        <v>236</v>
       </c>
       <c r="C10" s="18">
         <v>700</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E10" s="21">
         <v>18</v>
@@ -10481,10 +10481,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" t="s">
         <v>251</v>
-      </c>
-      <c r="B11" t="s">
-        <v>252</v>
       </c>
       <c r="C11" s="18">
         <v>700</v>
@@ -10534,10 +10534,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
         <v>223</v>
-      </c>
-      <c r="B12" t="s">
-        <v>224</v>
       </c>
       <c r="C12" s="18">
         <v>800</v>
@@ -10587,10 +10587,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" t="s">
         <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>222</v>
       </c>
       <c r="C13" s="18">
         <v>1400</v>
@@ -10640,10 +10640,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" t="s">
         <v>249</v>
-      </c>
-      <c r="B14" t="s">
-        <v>250</v>
       </c>
       <c r="C14" s="18">
         <v>1000</v>
@@ -10693,10 +10693,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" t="s">
         <v>233</v>
-      </c>
-      <c r="B15" t="s">
-        <v>234</v>
       </c>
       <c r="C15" s="18">
         <v>1100</v>
@@ -10746,10 +10746,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" t="s">
         <v>259</v>
-      </c>
-      <c r="B16" t="s">
-        <v>260</v>
       </c>
       <c r="C16" s="18">
         <v>1100</v>
@@ -10799,10 +10799,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" t="s">
         <v>255</v>
-      </c>
-      <c r="B17" t="s">
-        <v>256</v>
       </c>
       <c r="C17" s="18">
         <v>1300</v>
@@ -10852,10 +10852,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18" t="s">
         <v>257</v>
-      </c>
-      <c r="B18" t="s">
-        <v>258</v>
       </c>
       <c r="C18" s="18">
         <v>1900</v>
@@ -10905,10 +10905,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" t="s">
         <v>243</v>
-      </c>
-      <c r="B19" t="s">
-        <v>244</v>
       </c>
       <c r="C19" s="18">
         <v>1400</v>
@@ -10958,10 +10958,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" t="s">
         <v>247</v>
-      </c>
-      <c r="B20" t="s">
-        <v>248</v>
       </c>
       <c r="C20" s="18">
         <v>5500</v>
@@ -10979,7 +10979,7 @@
         <v>180</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J20" s="19" t="str">
         <f t="shared" si="0"/>
@@ -11011,16 +11011,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
         <v>241</v>
-      </c>
-      <c r="B21" t="s">
-        <v>242</v>
       </c>
       <c r="C21" s="18">
         <v>500</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E21" s="16">
         <v>35</v>
@@ -11032,7 +11032,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I21" s="5">
         <v>100</v>
@@ -11065,15 +11065,15 @@
         <v>130.5</v>
       </c>
       <c r="Q21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C22" s="18">
         <v>800</v>
@@ -11091,10 +11091,10 @@
         <v>50</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J22" s="19" t="str">
         <f t="shared" si="0"/>
@@ -11126,10 +11126,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C23" s="18">
         <v>250</v>
@@ -11150,7 +11150,7 @@
         <v>500</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J23" s="19" t="str">
         <f t="shared" si="0"/>
@@ -11182,10 +11182,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C24" s="18">
         <v>350</v>
@@ -11206,7 +11206,7 @@
         <v>1000</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J24" s="19" t="str">
         <f t="shared" si="0"/>
@@ -11238,7 +11238,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
@@ -11260,7 +11260,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D26" s="16">
         <v>1</v>
@@ -11279,7 +11279,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D27">
         <f t="shared" ref="D27:J27" si="6">SUM(D7:D9)</f>
@@ -11330,14 +11330,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>181</v>
@@ -11349,10 +11349,10 @@
         <v>183</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11377,7 +11377,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4">
         <f>7/45</f>
@@ -11401,14 +11401,14 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>181</v>
@@ -11420,10 +11420,10 @@
         <v>183</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -11448,7 +11448,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" s="4">
         <f>18/60</f>
@@ -11489,7 +11489,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -11512,10 +11512,10 @@
         <v>170</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11576,10 +11576,10 @@
         <v>170</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -11643,10 +11643,10 @@
         <v>170</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -11713,10 +11713,10 @@
         <v>170</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
HW1 Spreadsheet updated with speeds
</commit_message>
<xml_diff>
--- a/Balance Info/HW1 Ideal Design.xlsx
+++ b/Balance Info/HW1 Ideal Design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="6" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Costs!$A$1:$F$162</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Health!$A$1:$L$162</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Research!$A$1:$M$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Speeds!$A$1:$H$162</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Tech Tree'!$A$1:$I$162</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="329">
   <si>
     <t>Hiig</t>
   </si>
@@ -682,9 +683,6 @@
     <t>This is really a shitty attempt to compare this… hw1 obviously needs to use ques for non-combat stuff too. Honestly just ignore this….</t>
   </si>
   <si>
-    <t>Speeds are already good.</t>
-  </si>
-  <si>
     <t>Cost b7</t>
   </si>
   <si>
@@ -1007,6 +1005,27 @@
   </si>
   <si>
     <t>15?</t>
+  </si>
+  <si>
+    <t>350*1.4</t>
+  </si>
+  <si>
+    <t>b7 Speed</t>
+  </si>
+  <si>
+    <t>b8 Speed</t>
+  </si>
+  <si>
+    <t>hw1c Speed</t>
+  </si>
+  <si>
+    <t>b7 Upgraded</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>same as assault frig</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1142,6 +1161,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1424,9 +1455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,19 +1471,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2365,7 +2396,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E86">
         <v>425</v>
@@ -3019,7 +3050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3437,7 +3468,7 @@
         <v>15</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D40" s="8">
         <v>45</v>
@@ -4318,7 +4349,7 @@
         <v>18</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D93" s="8">
         <v>20</v>
@@ -5097,19 +5128,3732 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H475"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>232</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2*1.25</f>
+        <v>290</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>232</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>178</v>
+      </c>
+      <c r="C4" s="4">
+        <f>B4*1.25</f>
+        <v>222.5</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>279</v>
+      </c>
+      <c r="C5" s="4">
+        <f>B5*1.4</f>
+        <v>390.59999999999997</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>450</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>79</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ref="D7:D8" si="0">B7*1.25</f>
+        <v>98.75</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>81</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>101.25</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>177</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>120</v>
+      </c>
+      <c r="D10" s="4">
+        <f>B10*1.25</f>
+        <v>150</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>161</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>161</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>230</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>600</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>125</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>250</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>348</v>
+      </c>
+      <c r="C18" s="4">
+        <f>B18*1.4</f>
+        <v>487.2</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <v>165</v>
+      </c>
+      <c r="C19" s="4">
+        <f>B19*1.25</f>
+        <v>206.25</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>125</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>230</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>230</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>233</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="D24" s="4">
+        <f>B24*1.25</f>
+        <v>50</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>600</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>600</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
+        <v>232</v>
+      </c>
+      <c r="C27" s="4">
+        <f>B27*1.25</f>
+        <v>290</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>276</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>225</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>512</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="D31" s="4">
+        <f>B31*1.25</f>
+        <v>25</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>15</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>600</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2">
+        <v>176</v>
+      </c>
+      <c r="C35" s="4">
+        <f>B35*1.25</f>
+        <v>220</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>190</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>206</v>
+      </c>
+      <c r="D37" s="4">
+        <f>B37/$B$37</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="8">
+        <v>325</v>
+      </c>
+      <c r="H37">
+        <f>G37/$G$37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>390</v>
+      </c>
+      <c r="D38" s="4">
+        <f>B38/$B$65</f>
+        <v>0.80082135523613962</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="8">
+        <v>750</v>
+      </c>
+      <c r="H38">
+        <f>G38/$G$65</f>
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>105</v>
+      </c>
+      <c r="D39" s="4">
+        <f>B39/$B$45</f>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8">
+        <v>300</v>
+      </c>
+      <c r="H39">
+        <f>G39/$G$45</f>
+        <v>0.95238095238095233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>430</v>
+      </c>
+      <c r="D40" s="4">
+        <f>B40/$B$65</f>
+        <v>0.88295687885010266</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8">
+        <v>775</v>
+      </c>
+      <c r="H40">
+        <f>G40/$G$65</f>
+        <v>0.88571428571428568</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>165</v>
+      </c>
+      <c r="E41" s="5">
+        <v>206</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="8">
+        <v>325</v>
+      </c>
+      <c r="H41" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>210</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>210</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
         <v>214</v>
       </c>
+      <c r="D44" s="4">
+        <f>B44/$B$65</f>
+        <v>0.43942505133470228</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8">
+        <v>385</v>
+      </c>
+      <c r="H44">
+        <f>G44/$G$65</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>155</v>
+      </c>
+      <c r="D45" s="4">
+        <f>B45/$B$45</f>
+        <v>1</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8">
+        <v>315</v>
+      </c>
+      <c r="H45">
+        <f>G45/$G$45</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>210</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>210</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>210</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>210</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>210</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>210</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>210</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53">
+        <v>210</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>210</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55">
+        <v>210</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56">
+        <v>210</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>210</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>210</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59">
+        <v>210</v>
+      </c>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <v>166</v>
+      </c>
+      <c r="D60" s="4">
+        <f>B60/$B$37</f>
+        <v>0.80582524271844658</v>
+      </c>
+      <c r="E60" s="25">
+        <v>206</v>
+      </c>
+      <c r="G60" s="8">
+        <v>325</v>
+      </c>
+      <c r="H60">
+        <f>G60/$G$37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>114</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="8">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>350</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63">
+        <v>245</v>
+      </c>
+      <c r="D63" s="4">
+        <f>B63/$B$63</f>
+        <v>1</v>
+      </c>
+      <c r="E63" s="5">
+        <v>290</v>
+      </c>
+      <c r="F63" s="4">
+        <f>E63/$E$63</f>
+        <v>1</v>
+      </c>
+      <c r="G63" s="8">
+        <v>520</v>
+      </c>
+      <c r="H63">
+        <f>G63/$G$63</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>115</v>
+      </c>
+      <c r="D64" s="4">
+        <f>B64/$B$45</f>
+        <v>0.74193548387096775</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="8">
+        <v>250</v>
+      </c>
+      <c r="H64">
+        <f>G64/$G$45</f>
+        <v>0.79365079365079361</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>487</v>
+      </c>
+      <c r="D65" s="4">
+        <f>B65/$B$65</f>
+        <v>1</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="8">
+        <v>875</v>
+      </c>
+      <c r="H65">
+        <f>G65/$G$65</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>165</v>
+      </c>
+      <c r="D66" s="4">
+        <f>B66/$B$37</f>
+        <v>0.80097087378640774</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="G66" s="8">
+        <v>300</v>
+      </c>
+      <c r="H66">
+        <f>G66/$G$37</f>
+        <v>0.92307692307692313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>285</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D68" si="1">B67/$B$63</f>
+        <v>1.1632653061224489</v>
+      </c>
+      <c r="E67" s="5">
+        <v>305</v>
+      </c>
+      <c r="F67" s="4">
+        <f t="shared" ref="F67:F68" si="2">E67/$E$63</f>
+        <v>1.0517241379310345</v>
+      </c>
+      <c r="G67" s="8">
+        <v>575</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H68" si="3">G67/$G$63</f>
+        <v>1.1057692307692308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>246</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0040816326530613</v>
+      </c>
+      <c r="E68" s="5">
+        <v>255</v>
+      </c>
+      <c r="F68" s="4">
+        <f t="shared" si="2"/>
+        <v>0.87931034482758619</v>
+      </c>
+      <c r="G68" s="8">
+        <v>425</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>0.81730769230769229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="2">
+        <v>145</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" ref="D69:D70" si="4">B69/$B$45</f>
+        <v>0.93548387096774188</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69" s="4"/>
+      <c r="G69" s="8">
+        <v>295</v>
+      </c>
+      <c r="H69">
+        <f t="shared" ref="H69:H70" si="5">G69/$G$45</f>
+        <v>0.93650793650793651</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>48</v>
+      </c>
+      <c r="D70" s="4">
+        <f t="shared" si="4"/>
+        <v>0.30967741935483872</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F70" s="4"/>
+      <c r="G70" s="8">
+        <v>50</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="5"/>
+        <v>0.15873015873015872</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>275</v>
+      </c>
+      <c r="D71" s="4">
+        <f>B71/$B$63</f>
+        <v>1.1224489795918366</v>
+      </c>
+      <c r="E71" s="5">
+        <v>320</v>
+      </c>
+      <c r="F71" s="4">
+        <f>E71/$E$63</f>
+        <v>1.103448275862069</v>
+      </c>
+      <c r="G71" s="8">
+        <v>695</v>
+      </c>
+      <c r="H71">
+        <f>G71/$G$63</f>
+        <v>1.3365384615384615</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>600</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="8">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>350</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F73" s="4"/>
+      <c r="G73" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <v>255</v>
+      </c>
+      <c r="D74" s="4">
+        <f>B74/$B$63</f>
+        <v>1.0408163265306123</v>
+      </c>
+      <c r="E74" s="5">
+        <v>290</v>
+      </c>
+      <c r="F74" s="4">
+        <f>E74/$E$63</f>
+        <v>1</v>
+      </c>
+      <c r="G74" s="8">
+        <v>500</v>
+      </c>
+      <c r="H74">
+        <f>G74/$G$63</f>
+        <v>0.96153846153846156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="2">
+        <v>155</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" s="8">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="2">
+        <v>155</v>
+      </c>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="2">
+        <v>155</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="2">
+        <v>155</v>
+      </c>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="2">
+        <v>155</v>
+      </c>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="2">
+        <v>155</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81">
+        <v>110</v>
+      </c>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>100</v>
+      </c>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83">
+        <v>255</v>
+      </c>
+      <c r="D83" s="4">
+        <f>B83/$B$63</f>
+        <v>1.0408163265306123</v>
+      </c>
+      <c r="E83" s="5">
+        <v>255</v>
+      </c>
+      <c r="F83" s="4">
+        <f>E83/$E$63</f>
+        <v>0.87931034482758619</v>
+      </c>
+      <c r="G83" s="8">
+        <v>425</v>
+      </c>
+      <c r="H83">
+        <f>G83/$G$63</f>
+        <v>0.81730769230769229</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84">
+        <v>490</v>
+      </c>
+      <c r="D84" s="4">
+        <f>B84/$B$65</f>
+        <v>1.0061601642710472</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F84" s="4"/>
+      <c r="G84" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H84">
+        <f>G84/$G$65</f>
+        <v>1.1428571428571428</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="2">
+        <v>155</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="8">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86">
+        <v>287</v>
+      </c>
+      <c r="D86" s="4">
+        <f>B86/$B$37</f>
+        <v>1.3932038834951457</v>
+      </c>
+      <c r="E86" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="G86" s="8">
+        <v>450</v>
+      </c>
+      <c r="H86">
+        <f>G86/$G$37</f>
+        <v>1.3846153846153846</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87">
+        <v>228</v>
+      </c>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88">
+        <v>206</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89">
+        <v>390</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90">
+        <v>105</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91">
+        <v>165</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92">
+        <v>214</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93">
+        <v>487</v>
+      </c>
+      <c r="D93" s="4">
+        <f>B93/$B$65</f>
+        <v>1</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="8">
+        <v>875</v>
+      </c>
+      <c r="H93">
+        <f>G93/$G$65</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94">
+        <v>155</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95">
+        <v>166</v>
+      </c>
+      <c r="D95" s="4">
+        <f>B95/$B$37</f>
+        <v>0.80582524271844658</v>
+      </c>
+      <c r="E95" s="25">
+        <v>206</v>
+      </c>
+      <c r="G95" s="8">
+        <v>325</v>
+      </c>
+      <c r="H95">
+        <f>G95/$G$37</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106">
+        <v>114</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107">
+        <v>350</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108">
+        <v>245</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109">
+        <v>115</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110">
+        <v>487</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111">
+        <v>165</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112">
+        <v>285</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113">
+        <v>246</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="2">
+        <v>145</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115">
+        <v>48</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>117</v>
+      </c>
+      <c r="B116">
+        <v>275</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117">
+        <v>600</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>119</v>
+      </c>
+      <c r="B118">
+        <v>350</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119">
+        <v>255</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" s="2">
+        <v>155</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" s="2">
+        <v>155</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122" s="2">
+        <v>155</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" s="2">
+        <v>155</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" s="2">
+        <v>155</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" s="2">
+        <v>155</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>127</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>128</v>
+      </c>
+      <c r="B127">
+        <v>110</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>129</v>
+      </c>
+      <c r="B128">
+        <v>100</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>130</v>
+      </c>
+      <c r="B129">
+        <v>255</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>131</v>
+      </c>
+      <c r="B130" t="s">
+        <v>322</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" s="2">
+        <v>155</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>133</v>
+      </c>
+      <c r="B132">
+        <v>287</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>134</v>
+      </c>
+      <c r="B133">
+        <v>228</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B134" s="2">
+        <v>176</v>
+      </c>
+      <c r="C134" s="4">
+        <f>B134*1.25</f>
+        <v>220</v>
+      </c>
+      <c r="E134" s="24"/>
+      <c r="G134" s="4"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B135" s="2">
+        <v>79</v>
+      </c>
+      <c r="D135" s="4">
+        <f>B135*1.25</f>
+        <v>98.75</v>
+      </c>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B136" s="2">
+        <v>279</v>
+      </c>
+      <c r="C136" s="4">
+        <f>B136*1.4</f>
+        <v>390.59999999999997</v>
+      </c>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" s="2">
+        <v>81</v>
+      </c>
+      <c r="D137" s="4">
+        <f>B137*1.25</f>
+        <v>101.25</v>
+      </c>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="2">
+        <v>230</v>
+      </c>
+      <c r="C138" s="4">
+        <f>B138*1.3</f>
+        <v>299</v>
+      </c>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" s="2">
+        <v>120</v>
+      </c>
+      <c r="D140" s="4">
+        <f>B140*1.25</f>
+        <v>150</v>
+      </c>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B141" s="2">
+        <v>165</v>
+      </c>
+      <c r="C141" s="4">
+        <f>B141*1.25</f>
+        <v>206.25</v>
+      </c>
+      <c r="E141" s="24"/>
+      <c r="G141" s="4"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>143</v>
+      </c>
+      <c r="B142" s="2">
+        <v>650</v>
+      </c>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B143">
+        <v>230</v>
+      </c>
+      <c r="C143" s="4">
+        <f>B143*1.25</f>
+        <v>287.5</v>
+      </c>
+      <c r="E143" s="24"/>
+      <c r="G143" s="4"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B144" s="2">
+        <v>348</v>
+      </c>
+      <c r="C144" s="4">
+        <f t="shared" ref="C144:C145" si="6">B144*1.4</f>
+        <v>487.2</v>
+      </c>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B145" s="2">
+        <v>279</v>
+      </c>
+      <c r="C145" s="4">
+        <f t="shared" si="6"/>
+        <v>390.59999999999997</v>
+      </c>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B146" s="2">
+        <v>231</v>
+      </c>
+      <c r="C146" s="4">
+        <f t="shared" ref="C146:C148" si="7">B146*1.3</f>
+        <v>300.3</v>
+      </c>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B147" s="2">
+        <v>233</v>
+      </c>
+      <c r="C147" s="4">
+        <f t="shared" si="7"/>
+        <v>302.90000000000003</v>
+      </c>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B148" s="2">
+        <v>231</v>
+      </c>
+      <c r="C148" s="4">
+        <f t="shared" si="7"/>
+        <v>300.3</v>
+      </c>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B149">
+        <v>40</v>
+      </c>
+      <c r="D149" s="4">
+        <f>B149*1.25</f>
+        <v>50</v>
+      </c>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>151</v>
+      </c>
+      <c r="B150">
+        <v>40</v>
+      </c>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>152</v>
+      </c>
+      <c r="B151">
+        <v>50</v>
+      </c>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>153</v>
+      </c>
+      <c r="B152">
+        <v>250</v>
+      </c>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>154</v>
+      </c>
+      <c r="B153">
+        <v>50</v>
+      </c>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>155</v>
+      </c>
+      <c r="B154">
+        <v>600</v>
+      </c>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>156</v>
+      </c>
+      <c r="B155">
+        <v>600</v>
+      </c>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>157</v>
+      </c>
+      <c r="B156">
+        <v>600</v>
+      </c>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>158</v>
+      </c>
+      <c r="B157">
+        <v>276</v>
+      </c>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>159</v>
+      </c>
+      <c r="B158">
+        <v>225</v>
+      </c>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B159">
+        <v>420</v>
+      </c>
+      <c r="C159" s="4">
+        <f>B159*1.4</f>
+        <v>588</v>
+      </c>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B160" s="2">
+        <v>20</v>
+      </c>
+      <c r="D160" s="4">
+        <f>B160*1.25</f>
+        <v>25</v>
+      </c>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>162</v>
+      </c>
+      <c r="B161">
+        <v>125</v>
+      </c>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>163</v>
+      </c>
+      <c r="B162">
+        <v>125</v>
+      </c>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+    </row>
+    <row r="177" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+    </row>
+    <row r="178" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+    </row>
+    <row r="179" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
+    </row>
+    <row r="180" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
+    </row>
+    <row r="181" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
+    </row>
+    <row r="182" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
+    </row>
+    <row r="183" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
+    </row>
+    <row r="184" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
+    </row>
+    <row r="185" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
+    </row>
+    <row r="186" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
+    </row>
+    <row r="187" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
+    </row>
+    <row r="188" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
+    </row>
+    <row r="189" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
+    </row>
+    <row r="190" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
+    </row>
+    <row r="191" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
+    </row>
+    <row r="192" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
+    </row>
+    <row r="193" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
+      <c r="G193" s="4"/>
+    </row>
+    <row r="194" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
+      <c r="G194" s="4"/>
+    </row>
+    <row r="195" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E195" s="4"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="4"/>
+    </row>
+    <row r="196" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E196" s="4"/>
+      <c r="F196" s="4"/>
+      <c r="G196" s="4"/>
+    </row>
+    <row r="197" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E197" s="4"/>
+      <c r="F197" s="4"/>
+      <c r="G197" s="4"/>
+    </row>
+    <row r="198" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E198" s="4"/>
+      <c r="F198" s="4"/>
+      <c r="G198" s="4"/>
+    </row>
+    <row r="199" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E199" s="4"/>
+      <c r="F199" s="4"/>
+      <c r="G199" s="4"/>
+    </row>
+    <row r="200" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E200" s="4"/>
+      <c r="F200" s="4"/>
+      <c r="G200" s="4"/>
+    </row>
+    <row r="201" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E201" s="4"/>
+      <c r="F201" s="4"/>
+      <c r="G201" s="4"/>
+    </row>
+    <row r="202" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E202" s="4"/>
+      <c r="F202" s="4"/>
+      <c r="G202" s="4"/>
+    </row>
+    <row r="203" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E203" s="4"/>
+      <c r="F203" s="4"/>
+      <c r="G203" s="4"/>
+    </row>
+    <row r="204" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E204" s="4"/>
+      <c r="F204" s="4"/>
+      <c r="G204" s="4"/>
+    </row>
+    <row r="205" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E205" s="4"/>
+      <c r="F205" s="4"/>
+      <c r="G205" s="4"/>
+    </row>
+    <row r="206" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E206" s="4"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="4"/>
+    </row>
+    <row r="207" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E207" s="4"/>
+      <c r="F207" s="4"/>
+      <c r="G207" s="4"/>
+    </row>
+    <row r="208" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E208" s="4"/>
+      <c r="F208" s="4"/>
+      <c r="G208" s="4"/>
+    </row>
+    <row r="209" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E209" s="4"/>
+      <c r="F209" s="4"/>
+      <c r="G209" s="4"/>
+    </row>
+    <row r="210" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E210" s="4"/>
+      <c r="F210" s="4"/>
+      <c r="G210" s="4"/>
+    </row>
+    <row r="211" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E211" s="4"/>
+      <c r="F211" s="4"/>
+      <c r="G211" s="4"/>
+    </row>
+    <row r="212" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E212" s="4"/>
+      <c r="F212" s="4"/>
+      <c r="G212" s="4"/>
+    </row>
+    <row r="213" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E213" s="4"/>
+      <c r="F213" s="4"/>
+      <c r="G213" s="4"/>
+    </row>
+    <row r="214" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E214" s="4"/>
+      <c r="F214" s="4"/>
+      <c r="G214" s="4"/>
+    </row>
+    <row r="215" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E215" s="4"/>
+      <c r="F215" s="4"/>
+      <c r="G215" s="4"/>
+    </row>
+    <row r="216" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E216" s="4"/>
+      <c r="F216" s="4"/>
+      <c r="G216" s="4"/>
+    </row>
+    <row r="217" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E217" s="4"/>
+      <c r="F217" s="4"/>
+      <c r="G217" s="4"/>
+    </row>
+    <row r="218" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E218" s="4"/>
+      <c r="F218" s="4"/>
+      <c r="G218" s="4"/>
+    </row>
+    <row r="219" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E219" s="4"/>
+      <c r="F219" s="4"/>
+      <c r="G219" s="4"/>
+    </row>
+    <row r="220" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E220" s="4"/>
+      <c r="F220" s="4"/>
+      <c r="G220" s="4"/>
+    </row>
+    <row r="221" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E221" s="4"/>
+      <c r="F221" s="4"/>
+      <c r="G221" s="4"/>
+    </row>
+    <row r="222" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E222" s="4"/>
+      <c r="F222" s="4"/>
+      <c r="G222" s="4"/>
+    </row>
+    <row r="223" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E223" s="4"/>
+      <c r="F223" s="4"/>
+      <c r="G223" s="4"/>
+    </row>
+    <row r="224" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E224" s="4"/>
+      <c r="F224" s="4"/>
+      <c r="G224" s="4"/>
+    </row>
+    <row r="225" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E225" s="4"/>
+      <c r="F225" s="4"/>
+      <c r="G225" s="4"/>
+    </row>
+    <row r="226" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E226" s="4"/>
+      <c r="F226" s="4"/>
+      <c r="G226" s="4"/>
+    </row>
+    <row r="227" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E227" s="4"/>
+      <c r="F227" s="4"/>
+      <c r="G227" s="4"/>
+    </row>
+    <row r="228" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E228" s="4"/>
+      <c r="F228" s="4"/>
+      <c r="G228" s="4"/>
+    </row>
+    <row r="229" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E229" s="4"/>
+      <c r="F229" s="4"/>
+      <c r="G229" s="4"/>
+    </row>
+    <row r="230" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E230" s="4"/>
+      <c r="F230" s="4"/>
+      <c r="G230" s="4"/>
+    </row>
+    <row r="231" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E231" s="4"/>
+      <c r="F231" s="4"/>
+      <c r="G231" s="4"/>
+    </row>
+    <row r="232" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E232" s="4"/>
+      <c r="F232" s="4"/>
+      <c r="G232" s="4"/>
+    </row>
+    <row r="233" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E233" s="4"/>
+      <c r="F233" s="4"/>
+      <c r="G233" s="4"/>
+    </row>
+    <row r="234" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E234" s="4"/>
+      <c r="F234" s="4"/>
+      <c r="G234" s="4"/>
+    </row>
+    <row r="235" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E235" s="4"/>
+      <c r="F235" s="4"/>
+      <c r="G235" s="4"/>
+    </row>
+    <row r="236" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E236" s="4"/>
+      <c r="F236" s="4"/>
+      <c r="G236" s="4"/>
+    </row>
+    <row r="237" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E237" s="4"/>
+      <c r="F237" s="4"/>
+      <c r="G237" s="4"/>
+    </row>
+    <row r="238" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E238" s="4"/>
+      <c r="F238" s="4"/>
+      <c r="G238" s="4"/>
+    </row>
+    <row r="239" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E239" s="4"/>
+      <c r="F239" s="4"/>
+      <c r="G239" s="4"/>
+    </row>
+    <row r="240" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E240" s="4"/>
+      <c r="F240" s="4"/>
+      <c r="G240" s="4"/>
+    </row>
+    <row r="241" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E241" s="4"/>
+      <c r="F241" s="4"/>
+      <c r="G241" s="4"/>
+    </row>
+    <row r="242" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E242" s="4"/>
+      <c r="F242" s="4"/>
+      <c r="G242" s="4"/>
+    </row>
+    <row r="243" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E243" s="4"/>
+      <c r="F243" s="4"/>
+      <c r="G243" s="4"/>
+    </row>
+    <row r="244" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E244" s="4"/>
+      <c r="F244" s="4"/>
+      <c r="G244" s="4"/>
+    </row>
+    <row r="245" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E245" s="4"/>
+      <c r="F245" s="4"/>
+      <c r="G245" s="4"/>
+    </row>
+    <row r="246" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E246" s="4"/>
+      <c r="F246" s="4"/>
+      <c r="G246" s="4"/>
+    </row>
+    <row r="247" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E247" s="4"/>
+      <c r="F247" s="4"/>
+      <c r="G247" s="4"/>
+    </row>
+    <row r="248" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E248" s="4"/>
+      <c r="F248" s="4"/>
+      <c r="G248" s="4"/>
+    </row>
+    <row r="249" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E249" s="4"/>
+      <c r="F249" s="4"/>
+      <c r="G249" s="4"/>
+    </row>
+    <row r="250" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E250" s="4"/>
+      <c r="F250" s="4"/>
+      <c r="G250" s="4"/>
+    </row>
+    <row r="251" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E251" s="4"/>
+      <c r="F251" s="4"/>
+      <c r="G251" s="4"/>
+    </row>
+    <row r="252" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E252" s="4"/>
+      <c r="F252" s="4"/>
+      <c r="G252" s="4"/>
+    </row>
+    <row r="253" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E253" s="4"/>
+      <c r="F253" s="4"/>
+      <c r="G253" s="4"/>
+    </row>
+    <row r="254" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E254" s="4"/>
+      <c r="F254" s="4"/>
+      <c r="G254" s="4"/>
+    </row>
+    <row r="255" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E255" s="4"/>
+      <c r="F255" s="4"/>
+      <c r="G255" s="4"/>
+    </row>
+    <row r="256" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E256" s="4"/>
+      <c r="F256" s="4"/>
+      <c r="G256" s="4"/>
+    </row>
+    <row r="257" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E257" s="4"/>
+      <c r="F257" s="4"/>
+      <c r="G257" s="4"/>
+    </row>
+    <row r="258" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E258" s="4"/>
+      <c r="F258" s="4"/>
+      <c r="G258" s="4"/>
+    </row>
+    <row r="259" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E259" s="4"/>
+      <c r="F259" s="4"/>
+      <c r="G259" s="4"/>
+    </row>
+    <row r="260" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E260" s="4"/>
+      <c r="F260" s="4"/>
+      <c r="G260" s="4"/>
+    </row>
+    <row r="261" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E261" s="4"/>
+      <c r="F261" s="4"/>
+      <c r="G261" s="4"/>
+    </row>
+    <row r="262" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E262" s="4"/>
+      <c r="F262" s="4"/>
+      <c r="G262" s="4"/>
+    </row>
+    <row r="263" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E263" s="4"/>
+      <c r="F263" s="4"/>
+      <c r="G263" s="4"/>
+    </row>
+    <row r="264" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E264" s="4"/>
+      <c r="F264" s="4"/>
+      <c r="G264" s="4"/>
+    </row>
+    <row r="265" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E265" s="4"/>
+      <c r="F265" s="4"/>
+      <c r="G265" s="4"/>
+    </row>
+    <row r="266" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E266" s="4"/>
+      <c r="F266" s="4"/>
+      <c r="G266" s="4"/>
+    </row>
+    <row r="267" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E267" s="4"/>
+      <c r="F267" s="4"/>
+      <c r="G267" s="4"/>
+    </row>
+    <row r="268" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E268" s="4"/>
+      <c r="F268" s="4"/>
+      <c r="G268" s="4"/>
+    </row>
+    <row r="269" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E269" s="4"/>
+      <c r="F269" s="4"/>
+      <c r="G269" s="4"/>
+    </row>
+    <row r="270" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E270" s="4"/>
+      <c r="F270" s="4"/>
+      <c r="G270" s="4"/>
+    </row>
+    <row r="271" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E271" s="4"/>
+      <c r="F271" s="4"/>
+      <c r="G271" s="4"/>
+    </row>
+    <row r="272" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E272" s="4"/>
+      <c r="F272" s="4"/>
+      <c r="G272" s="4"/>
+    </row>
+    <row r="273" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E273" s="4"/>
+      <c r="F273" s="4"/>
+      <c r="G273" s="4"/>
+    </row>
+    <row r="274" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E274" s="4"/>
+      <c r="F274" s="4"/>
+      <c r="G274" s="4"/>
+    </row>
+    <row r="275" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E275" s="4"/>
+      <c r="F275" s="4"/>
+      <c r="G275" s="4"/>
+    </row>
+    <row r="276" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E276" s="4"/>
+      <c r="F276" s="4"/>
+      <c r="G276" s="4"/>
+    </row>
+    <row r="277" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E277" s="4"/>
+      <c r="F277" s="4"/>
+      <c r="G277" s="4"/>
+    </row>
+    <row r="278" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E278" s="4"/>
+      <c r="F278" s="4"/>
+      <c r="G278" s="4"/>
+    </row>
+    <row r="279" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E279" s="4"/>
+      <c r="F279" s="4"/>
+      <c r="G279" s="4"/>
+    </row>
+    <row r="280" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E280" s="4"/>
+      <c r="F280" s="4"/>
+      <c r="G280" s="4"/>
+    </row>
+    <row r="281" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E281" s="4"/>
+      <c r="F281" s="4"/>
+      <c r="G281" s="4"/>
+    </row>
+    <row r="282" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E282" s="4"/>
+      <c r="F282" s="4"/>
+      <c r="G282" s="4"/>
+    </row>
+    <row r="283" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E283" s="4"/>
+      <c r="F283" s="4"/>
+      <c r="G283" s="4"/>
+    </row>
+    <row r="284" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E284" s="4"/>
+      <c r="F284" s="4"/>
+      <c r="G284" s="4"/>
+    </row>
+    <row r="285" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E285" s="4"/>
+      <c r="F285" s="4"/>
+      <c r="G285" s="4"/>
+    </row>
+    <row r="286" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E286" s="4"/>
+      <c r="F286" s="4"/>
+      <c r="G286" s="4"/>
+    </row>
+    <row r="287" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E287" s="4"/>
+      <c r="F287" s="4"/>
+      <c r="G287" s="4"/>
+    </row>
+    <row r="288" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E288" s="4"/>
+      <c r="F288" s="4"/>
+      <c r="G288" s="4"/>
+    </row>
+    <row r="289" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E289" s="4"/>
+      <c r="F289" s="4"/>
+      <c r="G289" s="4"/>
+    </row>
+    <row r="290" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E290" s="4"/>
+      <c r="F290" s="4"/>
+      <c r="G290" s="4"/>
+    </row>
+    <row r="291" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E291" s="4"/>
+      <c r="F291" s="4"/>
+      <c r="G291" s="4"/>
+    </row>
+    <row r="292" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E292" s="4"/>
+      <c r="F292" s="4"/>
+      <c r="G292" s="4"/>
+    </row>
+    <row r="293" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E293" s="4"/>
+      <c r="F293" s="4"/>
+      <c r="G293" s="4"/>
+    </row>
+    <row r="294" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E294" s="4"/>
+      <c r="F294" s="4"/>
+      <c r="G294" s="4"/>
+    </row>
+    <row r="295" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E295" s="4"/>
+      <c r="F295" s="4"/>
+      <c r="G295" s="4"/>
+    </row>
+    <row r="296" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E296" s="4"/>
+      <c r="F296" s="4"/>
+      <c r="G296" s="4"/>
+    </row>
+    <row r="297" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E297" s="4"/>
+      <c r="F297" s="4"/>
+      <c r="G297" s="4"/>
+    </row>
+    <row r="298" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E298" s="4"/>
+      <c r="F298" s="4"/>
+      <c r="G298" s="4"/>
+    </row>
+    <row r="299" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E299" s="4"/>
+      <c r="F299" s="4"/>
+      <c r="G299" s="4"/>
+    </row>
+    <row r="300" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E300" s="4"/>
+      <c r="F300" s="4"/>
+      <c r="G300" s="4"/>
+    </row>
+    <row r="301" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E301" s="4"/>
+      <c r="F301" s="4"/>
+      <c r="G301" s="4"/>
+    </row>
+    <row r="302" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E302" s="4"/>
+      <c r="F302" s="4"/>
+      <c r="G302" s="4"/>
+    </row>
+    <row r="303" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E303" s="4"/>
+      <c r="F303" s="4"/>
+      <c r="G303" s="4"/>
+    </row>
+    <row r="304" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E304" s="4"/>
+      <c r="F304" s="4"/>
+      <c r="G304" s="4"/>
+    </row>
+    <row r="305" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E305" s="4"/>
+      <c r="F305" s="4"/>
+      <c r="G305" s="4"/>
+    </row>
+    <row r="306" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E306" s="4"/>
+      <c r="F306" s="4"/>
+      <c r="G306" s="4"/>
+    </row>
+    <row r="307" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E307" s="4"/>
+      <c r="F307" s="4"/>
+      <c r="G307" s="4"/>
+    </row>
+    <row r="308" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E308" s="4"/>
+      <c r="F308" s="4"/>
+      <c r="G308" s="4"/>
+    </row>
+    <row r="309" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E309" s="4"/>
+      <c r="F309" s="4"/>
+      <c r="G309" s="4"/>
+    </row>
+    <row r="310" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E310" s="4"/>
+      <c r="F310" s="4"/>
+      <c r="G310" s="4"/>
+    </row>
+    <row r="311" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E311" s="4"/>
+      <c r="F311" s="4"/>
+      <c r="G311" s="4"/>
+    </row>
+    <row r="312" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E312" s="4"/>
+      <c r="F312" s="4"/>
+      <c r="G312" s="4"/>
+    </row>
+    <row r="313" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E313" s="4"/>
+      <c r="F313" s="4"/>
+      <c r="G313" s="4"/>
+    </row>
+    <row r="314" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E314" s="4"/>
+      <c r="F314" s="4"/>
+      <c r="G314" s="4"/>
+    </row>
+    <row r="315" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E315" s="4"/>
+      <c r="F315" s="4"/>
+      <c r="G315" s="4"/>
+    </row>
+    <row r="316" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E316" s="4"/>
+      <c r="F316" s="4"/>
+      <c r="G316" s="4"/>
+    </row>
+    <row r="317" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E317" s="4"/>
+      <c r="F317" s="4"/>
+      <c r="G317" s="4"/>
+    </row>
+    <row r="318" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E318" s="4"/>
+      <c r="F318" s="4"/>
+      <c r="G318" s="4"/>
+    </row>
+    <row r="319" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E319" s="4"/>
+      <c r="F319" s="4"/>
+      <c r="G319" s="4"/>
+    </row>
+    <row r="320" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E320" s="4"/>
+      <c r="F320" s="4"/>
+      <c r="G320" s="4"/>
+    </row>
+    <row r="321" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E321" s="4"/>
+      <c r="F321" s="4"/>
+      <c r="G321" s="4"/>
+    </row>
+    <row r="322" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E322" s="4"/>
+      <c r="F322" s="4"/>
+      <c r="G322" s="4"/>
+    </row>
+    <row r="323" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E323" s="4"/>
+      <c r="F323" s="4"/>
+      <c r="G323" s="4"/>
+    </row>
+    <row r="324" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E324" s="24"/>
+      <c r="G324" s="4"/>
+    </row>
+    <row r="325" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E325" s="24"/>
+      <c r="G325" s="4"/>
+    </row>
+    <row r="326" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E326" s="24"/>
+      <c r="G326" s="4"/>
+    </row>
+    <row r="327" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E327" s="24"/>
+      <c r="G327" s="4"/>
+    </row>
+    <row r="328" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E328" s="24"/>
+      <c r="G328" s="4"/>
+    </row>
+    <row r="329" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E329" s="24"/>
+      <c r="G329" s="4"/>
+    </row>
+    <row r="330" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E330" s="24"/>
+      <c r="G330" s="4"/>
+    </row>
+    <row r="331" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E331" s="24"/>
+      <c r="G331" s="4"/>
+    </row>
+    <row r="332" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E332" s="24"/>
+      <c r="G332" s="4"/>
+    </row>
+    <row r="333" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E333" s="24"/>
+      <c r="G333" s="4"/>
+    </row>
+    <row r="334" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E334" s="24"/>
+      <c r="G334" s="4"/>
+    </row>
+    <row r="335" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E335" s="24"/>
+      <c r="G335" s="4"/>
+    </row>
+    <row r="336" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E336" s="24"/>
+      <c r="G336" s="4"/>
+    </row>
+    <row r="337" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E337" s="24"/>
+      <c r="G337" s="4"/>
+    </row>
+    <row r="338" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E338" s="24"/>
+      <c r="G338" s="4"/>
+    </row>
+    <row r="339" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E339" s="24"/>
+      <c r="G339" s="4"/>
+    </row>
+    <row r="340" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E340" s="24"/>
+      <c r="G340" s="4"/>
+    </row>
+    <row r="341" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E341" s="24"/>
+      <c r="G341" s="4"/>
+    </row>
+    <row r="342" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E342" s="24"/>
+      <c r="G342" s="4"/>
+    </row>
+    <row r="343" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E343" s="24"/>
+      <c r="G343" s="4"/>
+    </row>
+    <row r="344" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E344" s="24"/>
+      <c r="G344" s="4"/>
+    </row>
+    <row r="345" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E345" s="24"/>
+      <c r="G345" s="4"/>
+    </row>
+    <row r="346" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E346" s="24"/>
+      <c r="G346" s="4"/>
+    </row>
+    <row r="347" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E347" s="24"/>
+      <c r="G347" s="4"/>
+    </row>
+    <row r="348" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E348" s="24"/>
+      <c r="G348" s="4"/>
+    </row>
+    <row r="349" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E349" s="24"/>
+      <c r="G349" s="4"/>
+    </row>
+    <row r="350" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E350" s="24"/>
+      <c r="G350" s="4"/>
+    </row>
+    <row r="351" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E351" s="24"/>
+      <c r="G351" s="4"/>
+    </row>
+    <row r="352" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E352" s="24"/>
+      <c r="G352" s="4"/>
+    </row>
+    <row r="353" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E353" s="24"/>
+      <c r="G353" s="4"/>
+    </row>
+    <row r="354" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E354" s="24"/>
+      <c r="G354" s="4"/>
+    </row>
+    <row r="355" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E355" s="24"/>
+      <c r="G355" s="4"/>
+    </row>
+    <row r="356" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E356" s="24"/>
+      <c r="G356" s="4"/>
+    </row>
+    <row r="357" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E357" s="24"/>
+      <c r="G357" s="4"/>
+    </row>
+    <row r="358" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E358" s="24"/>
+      <c r="G358" s="4"/>
+    </row>
+    <row r="359" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E359" s="24"/>
+      <c r="G359" s="4"/>
+    </row>
+    <row r="360" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E360" s="24"/>
+      <c r="G360" s="4"/>
+    </row>
+    <row r="361" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E361" s="24"/>
+      <c r="G361" s="4"/>
+    </row>
+    <row r="362" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E362" s="24"/>
+      <c r="G362" s="4"/>
+    </row>
+    <row r="363" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E363" s="24"/>
+      <c r="G363" s="4"/>
+    </row>
+    <row r="364" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E364" s="24"/>
+      <c r="G364" s="4"/>
+    </row>
+    <row r="365" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E365" s="24"/>
+      <c r="G365" s="4"/>
+    </row>
+    <row r="366" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E366" s="24"/>
+      <c r="G366" s="4"/>
+    </row>
+    <row r="367" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E367" s="24"/>
+      <c r="G367" s="4"/>
+    </row>
+    <row r="368" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E368" s="24"/>
+      <c r="G368" s="4"/>
+    </row>
+    <row r="369" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E369" s="24"/>
+      <c r="G369" s="4"/>
+    </row>
+    <row r="370" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E370" s="24"/>
+      <c r="G370" s="4"/>
+    </row>
+    <row r="371" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E371" s="24"/>
+      <c r="G371" s="4"/>
+    </row>
+    <row r="372" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E372" s="24"/>
+      <c r="G372" s="4"/>
+    </row>
+    <row r="373" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E373" s="24"/>
+      <c r="G373" s="4"/>
+    </row>
+    <row r="374" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E374" s="24"/>
+      <c r="G374" s="4"/>
+    </row>
+    <row r="375" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E375" s="24"/>
+      <c r="G375" s="4"/>
+    </row>
+    <row r="376" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E376" s="24"/>
+      <c r="G376" s="4"/>
+    </row>
+    <row r="377" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E377" s="24"/>
+      <c r="G377" s="4"/>
+    </row>
+    <row r="378" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E378" s="24"/>
+      <c r="G378" s="4"/>
+    </row>
+    <row r="379" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E379" s="24"/>
+      <c r="G379" s="4"/>
+    </row>
+    <row r="380" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E380" s="24"/>
+      <c r="G380" s="4"/>
+    </row>
+    <row r="381" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E381" s="24"/>
+      <c r="G381" s="4"/>
+    </row>
+    <row r="382" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E382" s="24"/>
+      <c r="G382" s="4"/>
+    </row>
+    <row r="383" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E383" s="24"/>
+      <c r="G383" s="4"/>
+    </row>
+    <row r="384" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E384" s="24"/>
+      <c r="G384" s="4"/>
+    </row>
+    <row r="385" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E385" s="24"/>
+      <c r="G385" s="4"/>
+    </row>
+    <row r="386" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E386" s="24"/>
+      <c r="G386" s="4"/>
+    </row>
+    <row r="387" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E387" s="24"/>
+      <c r="G387" s="4"/>
+    </row>
+    <row r="388" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E388" s="24"/>
+      <c r="G388" s="4"/>
+    </row>
+    <row r="389" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E389" s="24"/>
+      <c r="G389" s="4"/>
+    </row>
+    <row r="390" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E390" s="24"/>
+      <c r="G390" s="4"/>
+    </row>
+    <row r="391" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E391" s="24"/>
+      <c r="G391" s="4"/>
+    </row>
+    <row r="392" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E392" s="24"/>
+      <c r="G392" s="4"/>
+    </row>
+    <row r="393" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E393" s="24"/>
+      <c r="G393" s="4"/>
+    </row>
+    <row r="394" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E394" s="24"/>
+      <c r="G394" s="4"/>
+    </row>
+    <row r="395" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E395" s="24"/>
+      <c r="G395" s="4"/>
+    </row>
+    <row r="396" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E396" s="24"/>
+      <c r="G396" s="4"/>
+    </row>
+    <row r="397" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E397" s="24"/>
+      <c r="G397" s="4"/>
+    </row>
+    <row r="398" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E398" s="24"/>
+      <c r="G398" s="4"/>
+    </row>
+    <row r="399" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E399" s="24"/>
+      <c r="G399" s="4"/>
+    </row>
+    <row r="400" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E400" s="24"/>
+      <c r="G400" s="4"/>
+    </row>
+    <row r="401" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E401" s="24"/>
+      <c r="G401" s="4"/>
+    </row>
+    <row r="402" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E402" s="24"/>
+      <c r="G402" s="4"/>
+    </row>
+    <row r="403" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E403" s="24"/>
+      <c r="G403" s="4"/>
+    </row>
+    <row r="404" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E404" s="24"/>
+      <c r="G404" s="4"/>
+    </row>
+    <row r="405" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E405" s="24"/>
+      <c r="G405" s="4"/>
+    </row>
+    <row r="406" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E406" s="24"/>
+      <c r="G406" s="4"/>
+    </row>
+    <row r="407" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E407" s="24"/>
+      <c r="G407" s="4"/>
+    </row>
+    <row r="408" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E408" s="24"/>
+      <c r="G408" s="4"/>
+    </row>
+    <row r="409" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E409" s="24"/>
+      <c r="G409" s="4"/>
+    </row>
+    <row r="410" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E410" s="24"/>
+      <c r="G410" s="4"/>
+    </row>
+    <row r="411" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E411" s="24"/>
+      <c r="G411" s="4"/>
+    </row>
+    <row r="412" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E412" s="24"/>
+      <c r="G412" s="4"/>
+    </row>
+    <row r="413" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E413" s="24"/>
+      <c r="G413" s="4"/>
+    </row>
+    <row r="414" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E414" s="24"/>
+      <c r="G414" s="4"/>
+    </row>
+    <row r="415" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E415" s="24"/>
+      <c r="G415" s="4"/>
+    </row>
+    <row r="416" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E416" s="24"/>
+      <c r="G416" s="4"/>
+    </row>
+    <row r="417" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E417" s="24"/>
+      <c r="G417" s="4"/>
+    </row>
+    <row r="418" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E418" s="24"/>
+      <c r="G418" s="4"/>
+    </row>
+    <row r="419" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E419" s="24"/>
+      <c r="G419" s="4"/>
+    </row>
+    <row r="420" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E420" s="24"/>
+      <c r="G420" s="4"/>
+    </row>
+    <row r="421" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E421" s="24"/>
+      <c r="G421" s="4"/>
+    </row>
+    <row r="422" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E422" s="24"/>
+      <c r="G422" s="4"/>
+    </row>
+    <row r="423" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E423" s="24"/>
+      <c r="G423" s="4"/>
+    </row>
+    <row r="424" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E424" s="24"/>
+      <c r="G424" s="4"/>
+    </row>
+    <row r="425" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E425" s="24"/>
+      <c r="G425" s="4"/>
+    </row>
+    <row r="426" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E426" s="24"/>
+      <c r="G426" s="4"/>
+    </row>
+    <row r="427" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E427" s="24"/>
+      <c r="G427" s="4"/>
+    </row>
+    <row r="428" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E428" s="24"/>
+      <c r="G428" s="4"/>
+    </row>
+    <row r="429" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E429" s="24"/>
+      <c r="G429" s="4"/>
+    </row>
+    <row r="430" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E430" s="24"/>
+      <c r="G430" s="4"/>
+    </row>
+    <row r="431" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E431" s="24"/>
+      <c r="G431" s="4"/>
+    </row>
+    <row r="432" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E432" s="24"/>
+      <c r="G432" s="4"/>
+    </row>
+    <row r="433" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E433" s="24"/>
+      <c r="G433" s="4"/>
+    </row>
+    <row r="434" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E434" s="24"/>
+      <c r="G434" s="4"/>
+    </row>
+    <row r="435" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E435" s="24"/>
+      <c r="G435" s="4"/>
+    </row>
+    <row r="436" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E436" s="24"/>
+      <c r="G436" s="4"/>
+    </row>
+    <row r="437" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E437" s="24"/>
+      <c r="G437" s="4"/>
+    </row>
+    <row r="438" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E438" s="24"/>
+      <c r="G438" s="4"/>
+    </row>
+    <row r="439" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E439" s="24"/>
+      <c r="G439" s="4"/>
+    </row>
+    <row r="440" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E440" s="24"/>
+      <c r="G440" s="4"/>
+    </row>
+    <row r="441" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E441" s="24"/>
+      <c r="G441" s="4"/>
+    </row>
+    <row r="442" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E442" s="24"/>
+      <c r="G442" s="4"/>
+    </row>
+    <row r="443" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E443" s="24"/>
+      <c r="G443" s="4"/>
+    </row>
+    <row r="444" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E444" s="24"/>
+      <c r="G444" s="4"/>
+    </row>
+    <row r="445" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E445" s="24"/>
+      <c r="G445" s="4"/>
+    </row>
+    <row r="446" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E446" s="24"/>
+      <c r="G446" s="4"/>
+    </row>
+    <row r="447" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E447" s="24"/>
+      <c r="G447" s="4"/>
+    </row>
+    <row r="448" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E448" s="24"/>
+      <c r="G448" s="4"/>
+    </row>
+    <row r="449" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E449" s="24"/>
+      <c r="G449" s="4"/>
+    </row>
+    <row r="450" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E450" s="24"/>
+      <c r="G450" s="4"/>
+    </row>
+    <row r="451" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E451" s="24"/>
+      <c r="G451" s="4"/>
+    </row>
+    <row r="452" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E452" s="24"/>
+      <c r="G452" s="4"/>
+    </row>
+    <row r="453" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E453" s="24"/>
+      <c r="G453" s="4"/>
+    </row>
+    <row r="454" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E454" s="24"/>
+      <c r="G454" s="4"/>
+    </row>
+    <row r="455" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E455" s="24"/>
+      <c r="G455" s="4"/>
+    </row>
+    <row r="456" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E456" s="24"/>
+      <c r="G456" s="4"/>
+    </row>
+    <row r="457" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E457" s="24"/>
+      <c r="G457" s="4"/>
+    </row>
+    <row r="458" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E458" s="24"/>
+      <c r="G458" s="4"/>
+    </row>
+    <row r="459" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E459" s="24"/>
+      <c r="G459" s="4"/>
+    </row>
+    <row r="460" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E460" s="24"/>
+      <c r="G460" s="4"/>
+    </row>
+    <row r="461" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E461" s="24"/>
+      <c r="G461" s="4"/>
+    </row>
+    <row r="462" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E462" s="24"/>
+      <c r="G462" s="4"/>
+    </row>
+    <row r="463" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E463" s="24"/>
+      <c r="G463" s="4"/>
+    </row>
+    <row r="464" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E464" s="24"/>
+      <c r="G464" s="4"/>
+    </row>
+    <row r="465" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E465" s="24"/>
+      <c r="G465" s="4"/>
+    </row>
+    <row r="466" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E466" s="24"/>
+      <c r="G466" s="4"/>
+    </row>
+    <row r="467" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E467" s="24"/>
+      <c r="G467" s="4"/>
+    </row>
+    <row r="468" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E468" s="24"/>
+      <c r="G468" s="4"/>
+    </row>
+    <row r="469" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E469" s="24"/>
+      <c r="G469" s="4"/>
+    </row>
+    <row r="470" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E470" s="24"/>
+      <c r="G470" s="4"/>
+    </row>
+    <row r="471" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E471" s="24"/>
+      <c r="G471" s="4"/>
+    </row>
+    <row r="472" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E472" s="24"/>
+      <c r="G472" s="4"/>
+    </row>
+    <row r="473" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E473" s="24"/>
+      <c r="G473" s="4"/>
+    </row>
+    <row r="474" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E474" s="24"/>
+      <c r="G474" s="4"/>
+    </row>
+    <row r="475" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E475" s="24"/>
+      <c r="G475" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H162"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5119,7 +8863,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5144,7 +8888,7 @@
         <v>206</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>205</v>
@@ -5162,7 +8906,7 @@
         <v>201</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7014,7 +10758,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K86" s="8">
         <v>12000</v>
@@ -8527,28 +12271,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>320</v>
-      </c>
       <c r="I1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -8560,7 +12304,7 @@
         <v>135</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8577,7 +12321,7 @@
         <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8588,7 +12332,7 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8609,7 +12353,7 @@
         <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8621,7 +12365,7 @@
         <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -8633,7 +12377,7 @@
         <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -8679,7 +12423,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -8691,7 +12435,7 @@
         <v>225</v>
       </c>
       <c r="E19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -8708,7 +12452,7 @@
         <v>225</v>
       </c>
       <c r="E21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -8725,7 +12469,7 @@
         <v>248</v>
       </c>
       <c r="E23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -8755,7 +12499,7 @@
         <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -8805,7 +12549,7 @@
         <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -8826,7 +12570,7 @@
         <v>190</v>
       </c>
       <c r="E37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F37" s="5">
         <v>160</v>
@@ -8841,7 +12585,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F38" s="5">
         <v>80</v>
@@ -8860,7 +12604,7 @@
         <v>248</v>
       </c>
       <c r="E39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F39" s="5">
         <v>200</v>
@@ -8875,7 +12619,7 @@
         <v>181</v>
       </c>
       <c r="E40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F40" s="5">
         <v>150</v>
@@ -8905,7 +12649,7 @@
         <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F44" s="5">
         <v>110</v>
@@ -8924,7 +12668,7 @@
         <v>369</v>
       </c>
       <c r="E45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F45" s="5">
         <v>390</v>
@@ -9013,7 +12757,7 @@
         <v>213</v>
       </c>
       <c r="E60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F60" s="5">
         <v>220</v>
@@ -9042,7 +12786,7 @@
         <v>185</v>
       </c>
       <c r="E63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F63" s="5">
         <v>160</v>
@@ -9061,7 +12805,7 @@
         <v>577</v>
       </c>
       <c r="E64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F64" s="5">
         <v>645</v>
@@ -9076,7 +12820,7 @@
         <v>110</v>
       </c>
       <c r="E65" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F65" s="5">
         <v>80</v>
@@ -9095,7 +12839,7 @@
         <v>242</v>
       </c>
       <c r="E66" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F66" s="5">
         <v>250</v>
@@ -9114,7 +12858,7 @@
         <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F67" s="5">
         <v>100</v>
@@ -9133,7 +12877,7 @@
         <v>213</v>
       </c>
       <c r="E68" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F68" s="5">
         <v>210</v>
@@ -9152,7 +12896,7 @@
         <v>283</v>
       </c>
       <c r="E69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F69" s="5">
         <v>270</v>
@@ -9179,7 +12923,7 @@
         <v>187</v>
       </c>
       <c r="E71" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F71" s="5">
         <v>170</v>
@@ -9262,7 +13006,7 @@
         <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F83" s="5">
         <v>140</v>
@@ -9297,7 +13041,7 @@
         <v>121</v>
       </c>
       <c r="E86" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F86" s="5">
         <v>100</v>
@@ -9357,7 +13101,7 @@
         <v>181</v>
       </c>
       <c r="E93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F93" s="5">
         <v>150</v>
@@ -9384,7 +13128,7 @@
         <v>213</v>
       </c>
       <c r="E95" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F95" s="5">
         <v>220</v>
@@ -9703,7 +13447,7 @@
         <v>212</v>
       </c>
       <c r="E134" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -9720,7 +13464,7 @@
         <v>63</v>
       </c>
       <c r="E136" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -9731,7 +13475,7 @@
         <v>70</v>
       </c>
       <c r="E137" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -9743,7 +13487,7 @@
         <v>160</v>
       </c>
       <c r="E138" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -9760,7 +13504,7 @@
         <v>169</v>
       </c>
       <c r="E140" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -9772,7 +13516,7 @@
         <v>180</v>
       </c>
       <c r="E141" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -9789,7 +13533,7 @@
         <v>222</v>
       </c>
       <c r="E143" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -9800,7 +13544,7 @@
         <v>45</v>
       </c>
       <c r="E144" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -9812,7 +13556,7 @@
         <v>63</v>
       </c>
       <c r="E145" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -9824,7 +13568,7 @@
         <v>160</v>
       </c>
       <c r="E146" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -9836,7 +13580,7 @@
         <v>188</v>
       </c>
       <c r="E147" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -9848,7 +13592,7 @@
         <v>118</v>
       </c>
       <c r="E148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -9951,60 +13695,60 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>264</v>
-      </c>
       <c r="E1" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="N1" t="s">
         <v>312</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="O1" t="s">
         <v>311</v>
       </c>
-      <c r="L1" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="P1" s="15" t="s">
         <v>314</v>
-      </c>
-      <c r="N1" t="s">
-        <v>313</v>
-      </c>
-      <c r="O1" t="s">
-        <v>312</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" t="s">
         <v>238</v>
-      </c>
-      <c r="B2" t="s">
-        <v>239</v>
       </c>
       <c r="C2" s="18">
         <v>100</v>
@@ -10052,15 +13796,15 @@
         <v>18.75</v>
       </c>
       <c r="Q2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" t="s">
         <v>236</v>
-      </c>
-      <c r="B3" t="s">
-        <v>237</v>
       </c>
       <c r="C3" s="18">
         <v>200</v>
@@ -10110,10 +13854,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
         <v>230</v>
-      </c>
-      <c r="B4" t="s">
-        <v>231</v>
       </c>
       <c r="C4" s="18">
         <v>400</v>
@@ -10163,10 +13907,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C5" s="18">
         <v>500</v>
@@ -10216,10 +13960,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C6" s="18">
         <v>500</v>
@@ -10269,10 +14013,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" t="s">
         <v>228</v>
-      </c>
-      <c r="B7" t="s">
-        <v>229</v>
       </c>
       <c r="C7" s="18">
         <v>800</v>
@@ -10322,10 +14066,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" t="s">
         <v>226</v>
-      </c>
-      <c r="B8" t="s">
-        <v>227</v>
       </c>
       <c r="C8" s="18">
         <v>900</v>
@@ -10375,16 +14119,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" t="s">
         <v>244</v>
-      </c>
-      <c r="B9" t="s">
-        <v>245</v>
       </c>
       <c r="C9" s="18">
         <v>600</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E9" s="21">
         <v>14</v>
@@ -10428,16 +14172,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" t="s">
         <v>234</v>
-      </c>
-      <c r="B10" t="s">
-        <v>235</v>
       </c>
       <c r="C10" s="18">
         <v>700</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E10" s="21">
         <v>18</v>
@@ -10481,10 +14225,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" t="s">
         <v>250</v>
-      </c>
-      <c r="B11" t="s">
-        <v>251</v>
       </c>
       <c r="C11" s="18">
         <v>700</v>
@@ -10534,10 +14278,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
         <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
       </c>
       <c r="C12" s="18">
         <v>800</v>
@@ -10587,10 +14331,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" t="s">
         <v>220</v>
-      </c>
-      <c r="B13" t="s">
-        <v>221</v>
       </c>
       <c r="C13" s="18">
         <v>1400</v>
@@ -10640,10 +14384,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" t="s">
         <v>248</v>
-      </c>
-      <c r="B14" t="s">
-        <v>249</v>
       </c>
       <c r="C14" s="18">
         <v>1000</v>
@@ -10693,10 +14437,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" t="s">
         <v>232</v>
-      </c>
-      <c r="B15" t="s">
-        <v>233</v>
       </c>
       <c r="C15" s="18">
         <v>1100</v>
@@ -10746,10 +14490,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" t="s">
         <v>258</v>
-      </c>
-      <c r="B16" t="s">
-        <v>259</v>
       </c>
       <c r="C16" s="18">
         <v>1100</v>
@@ -10799,10 +14543,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" t="s">
         <v>254</v>
-      </c>
-      <c r="B17" t="s">
-        <v>255</v>
       </c>
       <c r="C17" s="18">
         <v>1300</v>
@@ -10852,10 +14596,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" t="s">
         <v>256</v>
-      </c>
-      <c r="B18" t="s">
-        <v>257</v>
       </c>
       <c r="C18" s="18">
         <v>1900</v>
@@ -10905,10 +14649,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" t="s">
         <v>242</v>
-      </c>
-      <c r="B19" t="s">
-        <v>243</v>
       </c>
       <c r="C19" s="18">
         <v>1400</v>
@@ -10958,10 +14702,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" t="s">
         <v>246</v>
-      </c>
-      <c r="B20" t="s">
-        <v>247</v>
       </c>
       <c r="C20" s="18">
         <v>5500</v>
@@ -11011,16 +14755,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21" t="s">
         <v>240</v>
-      </c>
-      <c r="B21" t="s">
-        <v>241</v>
       </c>
       <c r="C21" s="18">
         <v>500</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E21" s="16">
         <v>35</v>
@@ -11065,15 +14809,15 @@
         <v>130.5</v>
       </c>
       <c r="Q21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C22" s="18">
         <v>800</v>
@@ -11126,10 +14870,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C23" s="18">
         <v>250</v>
@@ -11182,10 +14926,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C24" s="18">
         <v>350</v>
@@ -11238,7 +14982,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
@@ -11260,7 +15004,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D26" s="16">
         <v>1</v>
@@ -11279,7 +15023,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27">
         <f t="shared" ref="D27:J27" si="6">SUM(D7:D9)</f>

</xml_diff>